<commit_message>
Scraping unit test for medreg doctors works. Added jobs/import_medreg_doctor
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Personen_20141014.xlsx
+++ b/test/data/xlsx/Personen_20141014.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="73">
   <si>
     <t>GLN Person</t>
   </si>
@@ -50,6 +50,66 @@
     <t>Bemerkung Selbstdispensation</t>
   </si>
   <si>
+    <t>7601000813282</t>
+  </si>
+  <si>
+    <t>ABANTO PAYER</t>
+  </si>
+  <si>
+    <t>Dora Carmela</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Aarau</t>
+  </si>
+  <si>
+    <t>Aargau</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Zahnärztin/Zahnarzt</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>1213</t>
+  </si>
+  <si>
+    <t>Onex</t>
+  </si>
+  <si>
+    <t>Genf</t>
+  </si>
+  <si>
+    <t>7601000254207</t>
+  </si>
+  <si>
+    <t>Züst</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>8753</t>
+  </si>
+  <si>
+    <t>Mollis</t>
+  </si>
+  <si>
+    <t>Glarus</t>
+  </si>
+  <si>
+    <t>Ärztin/Arzt</t>
+  </si>
+  <si>
     <t>7601000186874</t>
   </si>
   <si>
@@ -68,18 +128,6 @@
     <t>Tessin</t>
   </si>
   <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>Ärztin/Arzt</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nein</t>
-  </si>
-  <si>
     <t>7601000201522</t>
   </si>
   <si>
@@ -105,12 +153,6 @@
   </si>
   <si>
     <t>Carouge</t>
-  </si>
-  <si>
-    <t>Genf</t>
-  </si>
-  <si>
-    <t>Zahnärztin/Zahnarzt</t>
   </si>
   <si>
     <t>7601000157638</t>
@@ -287,15 +329,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="555" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="480" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="7:13"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -347,7 +389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>11</v>
       </c>
@@ -379,24 +421,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>25</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>17</v>
@@ -408,97 +450,97 @@
         <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="G4" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="F5" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="0" t="s">
-        <v>42</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>19</v>
@@ -509,22 +551,22 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>17</v>
@@ -541,92 +583,92 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>19</v>
@@ -637,28 +679,28 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>19</v>
@@ -669,28 +711,28 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>19</v>
@@ -701,33 +743,129 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="0" t="s">
+      <c r="G16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="0" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix creating doctors, companies and addresses.
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Personen_20141014.xlsx
+++ b/test/data/xlsx/Personen_20141014.xlsx
@@ -155,24 +155,6 @@
     <t>Carouge</t>
   </si>
   <si>
-    <t>7601000157638</t>
-  </si>
-  <si>
-    <t>à Wengen</t>
-  </si>
-  <si>
-    <t>Daniel F.</t>
-  </si>
-  <si>
-    <t>4102</t>
-  </si>
-  <si>
-    <t>Binningen</t>
-  </si>
-  <si>
-    <t>Basel-Land</t>
-  </si>
-  <si>
     <t>7601000268969</t>
   </si>
   <si>
@@ -234,6 +216,24 @@
   </si>
   <si>
     <t>Münsterlingen</t>
+  </si>
+  <si>
+    <t>7601000010735</t>
+  </si>
+  <si>
+    <t>Cevey</t>
+  </si>
+  <si>
+    <t>Philippe Marc</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Neuchâtel</t>
+  </si>
+  <si>
+    <t>Neuenburg</t>
   </si>
 </sst>
 </file>
@@ -332,12 +332,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="480" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="1095" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:8"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -642,27 +642,27 @@
         <v>19</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>17</v>
@@ -679,22 +679,22 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="E11" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>17</v>
@@ -711,22 +711,22 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G12" s="0" t="s">
         <v>17</v>
@@ -743,22 +743,22 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>62</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G13" s="0" t="s">
         <v>17</v>
@@ -775,22 +775,22 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C14" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="E14" s="0" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G14" s="0" t="s">
         <v>17</v>
@@ -807,22 +807,22 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>67</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>17</v>
@@ -839,23 +839,23 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="C16" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="D16" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="F16" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G16" s="0" t="s">
         <v>17</v>
       </c>
@@ -869,6 +869,7 @@
         <v>20</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added fix for doctor with austrian additional qualification
</commit_message>
<xml_diff>
--- a/test/data/xlsx/Personen_20141014.xlsx
+++ b/test/data/xlsx/Personen_20141014.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="79">
   <si>
     <t>GLN Person</t>
   </si>
@@ -50,6 +50,186 @@
     <t>Bemerkung Selbstdispensation</t>
   </si>
   <si>
+    <t>7601000010735</t>
+  </si>
+  <si>
+    <t>Cevey</t>
+  </si>
+  <si>
+    <t>Philippe Marc</t>
+  </si>
+  <si>
+    <t>2000</t>
+  </si>
+  <si>
+    <t>Neuchâtel</t>
+  </si>
+  <si>
+    <t>Neuenburg</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>Ärztin/Arzt</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>7601000019080</t>
+  </si>
+  <si>
+    <t>Zwingli</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>1110</t>
+  </si>
+  <si>
+    <t>Morges</t>
+  </si>
+  <si>
+    <t>Waadt</t>
+  </si>
+  <si>
+    <t>1007</t>
+  </si>
+  <si>
+    <t>Lausanne</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>Lausanne 7</t>
+  </si>
+  <si>
+    <t>7601000078261</t>
+  </si>
+  <si>
+    <t>Kutschera</t>
+  </si>
+  <si>
+    <t>Harald</t>
+  </si>
+  <si>
+    <t>6221</t>
+  </si>
+  <si>
+    <t>Rickenbach LU</t>
+  </si>
+  <si>
+    <t>Luzern</t>
+  </si>
+  <si>
+    <t>7601000186874</t>
+  </si>
+  <si>
+    <t>a Marca</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>6925</t>
+  </si>
+  <si>
+    <t>Gentilino</t>
+  </si>
+  <si>
+    <t>Tessin</t>
+  </si>
+  <si>
+    <t>7601000201522</t>
+  </si>
+  <si>
+    <t>à Porta</t>
+  </si>
+  <si>
+    <t>Andry</t>
+  </si>
+  <si>
+    <t>8002</t>
+  </si>
+  <si>
+    <t>Zürich</t>
+  </si>
+  <si>
+    <t>7601000239730</t>
+  </si>
+  <si>
+    <t>Zwisler</t>
+  </si>
+  <si>
+    <t>Christoph Michael</t>
+  </si>
+  <si>
+    <t>8596</t>
+  </si>
+  <si>
+    <t>Münsterlingen</t>
+  </si>
+  <si>
+    <t>Thurgau</t>
+  </si>
+  <si>
+    <t>7601000254207</t>
+  </si>
+  <si>
+    <t>Züst</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>8753</t>
+  </si>
+  <si>
+    <t>Mollis</t>
+  </si>
+  <si>
+    <t>Glarus</t>
+  </si>
+  <si>
+    <t>7601000268969</t>
+  </si>
+  <si>
+    <t>à Wengen-Dörig</t>
+  </si>
+  <si>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>9220</t>
+  </si>
+  <si>
+    <t>Bischofszell</t>
+  </si>
+  <si>
+    <t>7601000295958</t>
+  </si>
+  <si>
+    <t>Christophe Eugène</t>
+  </si>
+  <si>
+    <t>1227</t>
+  </si>
+  <si>
+    <t>Carouge</t>
+  </si>
+  <si>
+    <t>Genf</t>
+  </si>
+  <si>
+    <t>Zahnärztin/Zahnarzt</t>
+  </si>
+  <si>
     <t>7601000813282</t>
   </si>
   <si>
@@ -68,172 +248,10 @@
     <t>Aargau</t>
   </si>
   <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>Zahnärztin/Zahnarzt</t>
-  </si>
-  <si>
-    <t>Ja</t>
-  </si>
-  <si>
-    <t>Nein</t>
-  </si>
-  <si>
     <t>1213</t>
   </si>
   <si>
     <t>Onex</t>
-  </si>
-  <si>
-    <t>Genf</t>
-  </si>
-  <si>
-    <t>7601000254207</t>
-  </si>
-  <si>
-    <t>Züst</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>8753</t>
-  </si>
-  <si>
-    <t>Mollis</t>
-  </si>
-  <si>
-    <t>Glarus</t>
-  </si>
-  <si>
-    <t>Ärztin/Arzt</t>
-  </si>
-  <si>
-    <t>7601000186874</t>
-  </si>
-  <si>
-    <t>a Marca</t>
-  </si>
-  <si>
-    <t>Luca</t>
-  </si>
-  <si>
-    <t>6925</t>
-  </si>
-  <si>
-    <t>Gentilino</t>
-  </si>
-  <si>
-    <t>Tessin</t>
-  </si>
-  <si>
-    <t>7601000201522</t>
-  </si>
-  <si>
-    <t>à Porta</t>
-  </si>
-  <si>
-    <t>Andry</t>
-  </si>
-  <si>
-    <t>8002</t>
-  </si>
-  <si>
-    <t>Zürich</t>
-  </si>
-  <si>
-    <t>7601000295958</t>
-  </si>
-  <si>
-    <t>Christophe Eugène</t>
-  </si>
-  <si>
-    <t>1227</t>
-  </si>
-  <si>
-    <t>Carouge</t>
-  </si>
-  <si>
-    <t>7601000268969</t>
-  </si>
-  <si>
-    <t>à Wengen-Dörig</t>
-  </si>
-  <si>
-    <t>Daniela</t>
-  </si>
-  <si>
-    <t>9220</t>
-  </si>
-  <si>
-    <t>Bischofszell</t>
-  </si>
-  <si>
-    <t>Thurgau</t>
-  </si>
-  <si>
-    <t>7601000019080</t>
-  </si>
-  <si>
-    <t>Zwingli</t>
-  </si>
-  <si>
-    <t>Martin</t>
-  </si>
-  <si>
-    <t>1110</t>
-  </si>
-  <si>
-    <t>Morges</t>
-  </si>
-  <si>
-    <t>Waadt</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>Lausanne</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>Lausanne 7</t>
-  </si>
-  <si>
-    <t>7601000239730</t>
-  </si>
-  <si>
-    <t>Zwisler</t>
-  </si>
-  <si>
-    <t>Christoph Michael</t>
-  </si>
-  <si>
-    <t>8596</t>
-  </si>
-  <si>
-    <t>Münsterlingen</t>
-  </si>
-  <si>
-    <t>7601000010735</t>
-  </si>
-  <si>
-    <t>Cevey</t>
-  </si>
-  <si>
-    <t>Philippe Marc</t>
-  </si>
-  <si>
-    <t>2000</t>
-  </si>
-  <si>
-    <t>Neuchâtel</t>
-  </si>
-  <si>
-    <t>Neuenburg</t>
   </si>
 </sst>
 </file>
@@ -335,9 +353,9 @@
   <dimension ref="A1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1095" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="960" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,22 +441,22 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G3" s="0" t="s">
         <v>17</v>
@@ -455,60 +473,60 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>29</v>
-      </c>
       <c r="G4" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>19</v>
@@ -519,54 +537,54 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="G6" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G7" s="0" t="s">
         <v>17</v>
@@ -583,92 +601,92 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="G9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G10" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>19</v>
@@ -679,60 +697,60 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G11" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="F12" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G12" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>19</v>
@@ -743,92 +761,92 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G13" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>57</v>
-      </c>
       <c r="G14" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="G15" s="0" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>19</v>
@@ -839,33 +857,65 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C16" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="G17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="0" t="s">
+      <c r="I17" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="0" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>